<commit_message>
Update data files for d1d2 diet
</commit_message>
<xml_diff>
--- a/Data/diet_test_rf.xlsx
+++ b/Data/diet_test_rf.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron.yerke\git\NHANES_Complexity\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E03C950-6F34-470E-9E00-82EC4F208900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{355861B4-2C08-4E77-B713-FDD85788622B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10180" xr2:uid="{78A4FAF4-B079-42A2-882B-DC6729F51F83}"/>
+    <workbookView xWindow="20" yWindow="620" windowWidth="19180" windowHeight="10180" xr2:uid="{78A4FAF4-B079-42A2-882B-DC6729F51F83}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="diet_test_rf" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>    d1_nutr_only_2015.csv,</t>
   </si>
@@ -53,9 +53,6 @@
     <t>    d1_nutri_food_2015.csv,</t>
   </si>
   <si>
-    <t>    d1_cat_g_2015.csv,</t>
-  </si>
-  <si>
     <t>    d1_nutri_cat_g_2015.csv,</t>
   </si>
   <si>
@@ -108,6 +105,42 @@
   </si>
   <si>
     <t>RF slurm</t>
+  </si>
+  <si>
+    <t>    d1d2_nutr_only_2015.csv,</t>
+  </si>
+  <si>
+    <t>    d1d2_food_g_2015.csv,</t>
+  </si>
+  <si>
+    <t>    d1d2_nutri_food_g_2015.csv,</t>
+  </si>
+  <si>
+    <t>    d1d2_food_2015.csv,</t>
+  </si>
+  <si>
+    <t>    d1d2_nutri_food_2015.csv,</t>
+  </si>
+  <si>
+    <t>    d1d2_cat_g_2015.csv,</t>
+  </si>
+  <si>
+    <t>    d1d2_nutri_cat_g_2015.csv,</t>
+  </si>
+  <si>
+    <t>    d1d2_cat_2015.csv,</t>
+  </si>
+  <si>
+    <t>    d1d2_nutri_cat_2015.csv,</t>
+  </si>
+  <si>
+    <t>    d1d2_nutri_food_g_cat_g_2015.csv,</t>
+  </si>
+  <si>
+    <t>    d1d2_nutri_food_cat_2015.csv,</t>
+  </si>
+  <si>
+    <t>d1_diet_orgs</t>
   </si>
 </sst>
 </file>
@@ -459,112 +492,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1318A4D4-C87D-471D-A451-7CBE0C72705F}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38.36328125" customWidth="1"/>
     <col min="2" max="2" width="47.08984375" customWidth="1"/>
+    <col min="3" max="3" width="29.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
         <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>